<commit_message>
+taskkill support +1C coloring for &
</commit_message>
<xml_diff>
--- a/Publication/Translators.xlsx
+++ b/Publication/Translators.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -61,6 +61,15 @@
   </si>
   <si>
     <t>bovirus@gmail.com</t>
+  </si>
+  <si>
+    <t>Dieter Hummel</t>
+  </si>
+  <si>
+    <t>German</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dh@level47.de </t>
   </si>
 </sst>
 </file>
@@ -432,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -499,15 +508,27 @@
         <v>14</v>
       </c>
     </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1"/>
     <hyperlink ref="C2" r:id="rId2"/>
     <hyperlink ref="C4" r:id="rId3"/>
     <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>